<commit_message>
complete README + some examples pt1
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
+    <sheet name="controlled vocabularies" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
   <si>
     <t>scientific_name</t>
   </si>
@@ -67,9 +68,6 @@
     <t>specifications</t>
   </si>
   <si>
-    <t>examples</t>
-  </si>
-  <si>
     <t>scientific name</t>
   </si>
   <si>
@@ -82,14 +80,295 @@
     <t>The full scientific name, with authorship and date information if known. This should be the name in lowest level taxonomic rank that can be determined.</t>
   </si>
   <si>
-    <t>Coleoptera, Ctenomys sociabilis, Ambystoma tigrinum diaboli, Roptrocerus typographi (Györfi, 1952) , Quercus agrifolia var. oxyadenia (Torr.) J.T. Howell</t>
+    <t>Plantae</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Fungi</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Archaea</t>
+  </si>
+  <si>
+    <t>Chromista</t>
+  </si>
+  <si>
+    <t>Protozoa</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>subgenus</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>subspecies</t>
+  </si>
+  <si>
+    <t>variety</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>recommended</t>
+  </si>
+  <si>
+    <t>The specific description of the place. This applies to a region, a city, a town, etc. This does not apply to the actual location that observations were made (so no coordinates)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The standard code for the country in which the taxon occurs. Recommended best practice is to use ISO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3166-1 alpha-2 country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> codes</t>
+    </r>
+  </si>
+  <si>
+    <t>The full scientific name of the kingdom in which the taxon is classified. The use of a controlled vocabulary is obligated</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The taxonomic rank of the scientific_name. The use of a controlled vocabulary is obligated. We use a subset of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Taxonomic Rank GBIF Vocabulary</t>
+    </r>
+  </si>
+  <si>
+    <t>A statement about the presence or absence of a taxon within the specified locality. The use of a controlled vocabulary is obligated. We use a subset of the Occurrence Status GBIF Vocabulary</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Subset </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Taxonomic Rank GBIF Vocabulary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>terms: genus, subgenus, species, subspecies, variety, form</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Subset </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Occurrence Status GBIF Vocabulary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> terms: present, absent, doubtful</t>
+    </r>
+  </si>
+  <si>
+    <t>Controlled vocabulary</t>
+  </si>
+  <si>
+    <t>Free overview of ISO 3166-1 alpha-2 codes</t>
+  </si>
+  <si>
+    <t>Official ISO standard website</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>doubtful</t>
+  </si>
+  <si>
+    <t>Threat status of a species as defined by IUCN</t>
+  </si>
+  <si>
+    <t>IUCN criteria categories</t>
+  </si>
+  <si>
+    <t>IUCN criteria</t>
+  </si>
+  <si>
+    <t>extinct</t>
+  </si>
+  <si>
+    <t>extinct in the wild</t>
+  </si>
+  <si>
+    <t>critically endangered</t>
+  </si>
+  <si>
+    <t>endangered</t>
+  </si>
+  <si>
+    <t>vulnerable</t>
+  </si>
+  <si>
+    <t>near threatened</t>
+  </si>
+  <si>
+    <t>least concern</t>
+  </si>
+  <si>
+    <t>data deficient</t>
+  </si>
+  <si>
+    <t>not evaluated</t>
+  </si>
+  <si>
+    <t>multipele, separated by a pipe ("|")</t>
+  </si>
+  <si>
+    <t>A bibliographic reference for the resource as a statement indicating how this record should be cited (attributed) when used. Recommended practice is to use the doi of the publication when provided. Otherwise, include the full bibliographic reference to identify the resource as unambiguously as possible. When no full bibliographic reference is available, use an URL when available. Multipele references should be separated using "|" as a separator.</t>
+  </si>
+  <si>
+    <t>Bassia laniflora (S.G. Gmel.) A.J. Scott</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Flanders</t>
+  </si>
+  <si>
+    <t>Verloove F (2018) Manual of Alien Plants of Belgium. Botanic Garden of Meise, Belgium. At: http://alienplantsbelgium.be.</t>
+  </si>
+  <si>
+    <t>Amaranthus macrocarpus Benth. var. pallidus Benth.</t>
+  </si>
+  <si>
+    <t>Walloon region</t>
+  </si>
+  <si>
+    <t>Alytes obstetricans</t>
+  </si>
+  <si>
+    <t>introduced</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
+    <t>Bauwens D &amp; Claus K (1996) Verspreiding van amfibieën en reptillen in Vlaanderen. De Wielewaal, Turnhout</t>
+  </si>
+  <si>
+    <t>Plebejus dardanus</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>Absent according to Rudi Verovnik</t>
+  </si>
+  <si>
+    <t>Euphorbia x pseudovirgata (Schur)</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10530-016-1278-z</t>
+  </si>
+  <si>
+    <t>Calamintha nepeta glandulosa</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>data based solely on DAISIE portal</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3897/neobiota.23.5665</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +380,39 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,20 +447,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal_Sheet1" xfId="2"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,61 +847,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="18.25" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="21.625" customWidth="1"/>
-    <col min="9" max="9" width="19.75" customWidth="1"/>
-    <col min="10" max="10" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="61.25" style="14" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="19.125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="18.25" style="14" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="14" customWidth="1"/>
+    <col min="6" max="6" width="22" style="14" customWidth="1"/>
+    <col min="7" max="7" width="23.875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="21.625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="82.75" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.875" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I7" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies'!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies'!$B$2:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies'!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies'!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -547,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,48 +1112,346 @@
     <col min="2" max="2" width="22.75" customWidth="1"/>
     <col min="3" max="3" width="15.75" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="78" customWidth="1"/>
+    <col min="5" max="5" width="86.75" customWidth="1"/>
     <col min="6" max="6" width="66.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>15</v>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" display="Taxonomic Rank GBIF Vocabulary"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F9" r:id="rId4" location="categories"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
       <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add multipele distributions per taxon to template file
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>scientific_name</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>https://doi.org/10.3897/neobiota.23.5665</t>
+  </si>
+  <si>
+    <t>French region</t>
   </si>
 </sst>
 </file>
@@ -463,12 +466,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -490,12 +487,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -508,6 +499,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -847,56 +850,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.25" style="14" customWidth="1"/>
-    <col min="2" max="2" width="21.875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="19.125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="14" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="14" customWidth="1"/>
-    <col min="6" max="6" width="22" style="14" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="82.75" style="14" customWidth="1"/>
-    <col min="10" max="10" width="14.875" style="14" customWidth="1"/>
-    <col min="11" max="16384" width="11" style="14"/>
+    <col min="1" max="1" width="61.25" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="19.125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.25" style="12" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22" style="12" customWidth="1"/>
+    <col min="7" max="7" width="23.875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21.625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="82.75" style="12" customWidth="1"/>
+    <col min="10" max="10" width="14.875" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -916,10 +919,10 @@
       <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="13" t="s">
         <v>67</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -927,139 +930,165 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="12" t="s">
         <v>67</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I5" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J7" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I8" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J8" s="17" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1"/>
-    <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="I8" r:id="rId1"/>
+    <hyperlink ref="I5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1155,164 +1184,164 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="13" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Delete kingdom & taxonRank from data template
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
   <si>
     <t>scientific_name</t>
   </si>
@@ -850,273 +850,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.25" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="19.125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="22" style="12" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="82.75" style="12" customWidth="1"/>
-    <col min="10" max="10" width="14.875" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="11" style="12"/>
+    <col min="2" max="2" width="18.25" style="12" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22" style="12" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="21.625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="82.75" style="12" customWidth="1"/>
+    <col min="8" max="8" width="14.875" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="E1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="G5" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="G8" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1"/>
-    <hyperlink ref="I5" r:id="rId2"/>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'controlled vocabularies'!$A$2:$A$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'controlled vocabularies'!$B$2:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled vocabularies'!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled vocabularies'!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove `Flanders` for one record
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>scientific_name</t>
   </si>
@@ -853,7 +853,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -997,9 +997,6 @@
       </c>
       <c r="C6" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Add taxon rank to raw data file
I think it's better to add this term to the raw data file as the GBIF nameparser sometimes renders errors (see https://github.com/gbif/name-parser/issues/26)
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
-    <sheet name="controlled vocabularies" sheetId="3" r:id="rId3"/>
+    <sheet name="controlled vocabularies (hide)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>scientific_name</t>
   </si>
@@ -455,7 +455,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -511,6 +511,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -850,56 +853,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.25" style="12" customWidth="1"/>
     <col min="2" max="2" width="32" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.25" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="21.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="82.75" style="12" customWidth="1"/>
-    <col min="9" max="9" width="14.875" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="12"/>
+    <col min="3" max="3" width="19.875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.25" style="12" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22" style="12" customWidth="1"/>
+    <col min="7" max="7" width="23.875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21.625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="82.75" style="12" customWidth="1"/>
+    <col min="10" max="10" width="14.875" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -907,176 +914,207 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="I8" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="J8" s="17" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
-    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="I8" r:id="rId1"/>
+    <hyperlink ref="I5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'controlled vocabularies'!$C$2:$C$4</xm:f>
+            <xm:f>'controlled vocabularies (hide)'!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'controlled vocabularies'!$D$2:$D$10</xm:f>
+            <xm:f>'controlled vocabularies (hide)'!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies (hide)'!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies (hide)'!$B$2:$B$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1092,7 +1130,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1364,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove taxon_rank column + add new taxa for nameparser function
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -12,6 +12,7 @@
     <sheet name="controlled vocabularies (hide)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
   <si>
     <t>scientific_name</t>
   </si>
@@ -365,6 +366,21 @@
   </si>
   <si>
     <t>French region</t>
+  </si>
+  <si>
+    <t>Cotoneaster x 'Hybridus pendulus'</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>Acmella agg.</t>
+  </si>
+  <si>
+    <t>AseroÙ rubra</t>
+  </si>
+  <si>
+    <t>Triticosecale x</t>
   </si>
 </sst>
 </file>
@@ -455,7 +471,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -511,9 +527,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -853,60 +866,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.25" style="12" customWidth="1"/>
     <col min="2" max="2" width="32" style="12" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="22" style="12" customWidth="1"/>
-    <col min="7" max="7" width="23.875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="82.75" style="12" customWidth="1"/>
-    <col min="10" max="10" width="14.875" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="11" style="12"/>
+    <col min="3" max="3" width="18.25" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="22" style="12" customWidth="1"/>
+    <col min="6" max="6" width="23.875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="21.625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="82.75" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14.875" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="E1" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="H1" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
@@ -914,207 +923,251 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="E2" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="F2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>30</v>
+      <c r="C3" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>30</v>
+      <c r="C4" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>74</v>
       </c>
+      <c r="E5" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>61</v>
       </c>
+      <c r="E6" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="F6" s="12" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>71</v>
       </c>
+      <c r="E7" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="F7" s="12" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>77</v>
       </c>
+      <c r="E8" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="F8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="H8" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="I8" s="17" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1"/>
-    <hyperlink ref="I5" r:id="rId2"/>
+    <hyperlink ref="H8" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled vocabularies (hide)'!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled vocabularies (hide)'!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled vocabularies (hide)'!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'controlled vocabularies (hide)'!$B$2:$B$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove taxon_rank information from README in raw_data
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -12,7 +12,6 @@
     <sheet name="controlled vocabularies (hide)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>scientific_name</t>
   </si>
@@ -159,59 +158,7 @@
     <t>The full scientific name of the kingdom in which the taxon is classified. The use of a controlled vocabulary is obligated</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The taxonomic rank of the scientific_name. The use of a controlled vocabulary is obligated. We use a subset of the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Taxonomic Rank GBIF Vocabulary</t>
-    </r>
-  </si>
-  <si>
     <t>A statement about the presence or absence of a taxon within the specified locality. The use of a controlled vocabulary is obligated. We use a subset of the Occurrence Status GBIF Vocabulary</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Subset </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Taxonomic Rank GBIF Vocabulary </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>terms: genus, subgenus, species, subspecies, variety, form</t>
-    </r>
   </si>
   <si>
     <r>
@@ -471,7 +418,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -491,12 +438,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -869,276 +810,276 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.25" style="12" customWidth="1"/>
-    <col min="2" max="2" width="32" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.25" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="21.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="82.75" style="12" customWidth="1"/>
-    <col min="9" max="9" width="14.875" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="12"/>
+    <col min="1" max="1" width="61.25" style="10" customWidth="1"/>
+    <col min="2" max="2" width="32" style="10" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22" style="10" customWidth="1"/>
+    <col min="6" max="6" width="23.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="21.625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="82.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.875" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="B3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="12" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="F8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="16" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="C9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>67</v>
+      <c r="C12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1180,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1154,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1252,59 +1193,57 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>36</v>
+      <c r="C4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -1312,17 +1251,19 @@
       <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>17</v>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1333,82 +1274,61 @@
       <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="Taxonomic Rank GBIF Vocabulary"/>
-    <hyperlink ref="F8" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4" location="categories"/>
+    <hyperlink ref="F7" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3" location="categories"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1438,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1449,10 +1369,10 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1463,10 +1383,10 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,10 +1397,10 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1491,7 +1411,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1502,7 +1422,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,7 +1433,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,17 +1441,17 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into add_recipe"
This reverts commit ef49473741554577888a9eaa260bdb2f4c6cba3c, reversing
changes made to 9ca5b67870fe7a454938c839a4d8a503468d2552.
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
+    <sheet name="controlled vocabularies (hide)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,9 +20,321 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
+  <si>
+    <t>scientific_name</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>taxon_rank</t>
+  </si>
+  <si>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>occurrence_status</t>
+  </si>
+  <si>
+    <t>establishment_means</t>
+  </si>
+  <si>
+    <t>threat_status</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>number of values allowed</t>
+  </si>
+  <si>
+    <t>obligatory</t>
+  </si>
+  <si>
+    <t>controlled vocabulary</t>
+  </si>
+  <si>
+    <t>specifications</t>
+  </si>
+  <si>
+    <t>scientific name</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>The full scientific name, with authorship and date information if known. This should be the name in lowest level taxonomic rank that can be determined.</t>
+  </si>
+  <si>
+    <t>Plantae</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Fungi</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Archaea</t>
+  </si>
+  <si>
+    <t>Chromista</t>
+  </si>
+  <si>
+    <t>Protozoa</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>subgenus</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>subspecies</t>
+  </si>
+  <si>
+    <t>variety</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>recommended</t>
+  </si>
+  <si>
+    <t>The specific description of the place. This applies to a region, a city, a town, etc. This does not apply to the actual location that observations were made (so no coordinates)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The standard code for the country in which the taxon occurs. Recommended best practice is to use ISO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3166-1 alpha-2 country</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> codes</t>
+    </r>
+  </si>
+  <si>
+    <t>The full scientific name of the kingdom in which the taxon is classified. The use of a controlled vocabulary is obligated</t>
+  </si>
+  <si>
+    <t>A statement about the presence or absence of a taxon within the specified locality. The use of a controlled vocabulary is obligated. We use a subset of the Occurrence Status GBIF Vocabulary</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Subset </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Occurrence Status GBIF Vocabulary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> terms: present, absent, doubtful</t>
+    </r>
+  </si>
+  <si>
+    <t>Controlled vocabulary</t>
+  </si>
+  <si>
+    <t>Free overview of ISO 3166-1 alpha-2 codes</t>
+  </si>
+  <si>
+    <t>Official ISO standard website</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>doubtful</t>
+  </si>
+  <si>
+    <t>Threat status of a species as defined by IUCN</t>
+  </si>
+  <si>
+    <t>IUCN criteria categories</t>
+  </si>
+  <si>
+    <t>IUCN criteria</t>
+  </si>
+  <si>
+    <t>extinct</t>
+  </si>
+  <si>
+    <t>extinct in the wild</t>
+  </si>
+  <si>
+    <t>critically endangered</t>
+  </si>
+  <si>
+    <t>endangered</t>
+  </si>
+  <si>
+    <t>vulnerable</t>
+  </si>
+  <si>
+    <t>near threatened</t>
+  </si>
+  <si>
+    <t>least concern</t>
+  </si>
+  <si>
+    <t>data deficient</t>
+  </si>
+  <si>
+    <t>not evaluated</t>
+  </si>
+  <si>
+    <t>multipele, separated by a pipe ("|")</t>
+  </si>
+  <si>
+    <t>A bibliographic reference for the resource as a statement indicating how this record should be cited (attributed) when used. Recommended practice is to use the doi of the publication when provided. Otherwise, include the full bibliographic reference to identify the resource as unambiguously as possible. When no full bibliographic reference is available, use an URL when available. Multipele references should be separated using "|" as a separator.</t>
+  </si>
+  <si>
+    <t>Bassia laniflora (S.G. Gmel.) A.J. Scott</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Flanders</t>
+  </si>
+  <si>
+    <t>Verloove F (2018) Manual of Alien Plants of Belgium. Botanic Garden of Meise, Belgium. At: http://alienplantsbelgium.be.</t>
+  </si>
+  <si>
+    <t>Amaranthus macrocarpus Benth. var. pallidus Benth.</t>
+  </si>
+  <si>
+    <t>Walloon region</t>
+  </si>
+  <si>
+    <t>Alytes obstetricans</t>
+  </si>
+  <si>
+    <t>introduced</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
+    <t>Bauwens D &amp; Claus K (1996) Verspreiding van amfibieën en reptillen in Vlaanderen. De Wielewaal, Turnhout</t>
+  </si>
+  <si>
+    <t>Plebejus dardanus</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>Absent according to Rudi Verovnik</t>
+  </si>
+  <si>
+    <t>Euphorbia x pseudovirgata (Schur)</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10530-016-1278-z</t>
+  </si>
+  <si>
+    <t>Calamintha nepeta glandulosa</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>data based solely on DAISIE portal</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3897/neobiota.23.5665</t>
+  </si>
+  <si>
+    <t>French region</t>
+  </si>
+  <si>
+    <t>Cotoneaster x 'Hybridus pendulus'</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>Acmella agg.</t>
+  </si>
+  <si>
+    <t>AseroÙ rubra</t>
+  </si>
+  <si>
+    <t>Triticosecale x</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -28,13 +342,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,17 +413,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal_Sheet1" xfId="2"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -382,17 +807,655 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.25" style="10" customWidth="1"/>
+    <col min="2" max="2" width="32" style="10" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="22" style="10" customWidth="1"/>
+    <col min="6" max="6" width="23.875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="21.625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="82.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.875" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies (hide)'!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies (hide)'!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'controlled vocabularies (hide)'!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="2" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="86.75" customWidth="1"/>
+    <col min="6" max="6" width="66.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3" location="categories"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update raw data with event date information
</commit_message>
<xml_diff>
--- a/data/raw/checklist.xlsx
+++ b/data/raw/checklist.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25605" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
     <sheet name="controlled vocabularies (hide)" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
   <si>
     <t>scientific_name</t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>Triticosecale x</t>
+  </si>
+  <si>
+    <t>start_year</t>
+  </si>
+  <si>
+    <t>end_year</t>
+  </si>
+  <si>
+    <t>must be ISO 8601 format using a 4-digit year (yyyy)</t>
   </si>
 </sst>
 </file>
@@ -807,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -819,15 +828,15 @@
     <col min="2" max="2" width="32" style="10" customWidth="1"/>
     <col min="3" max="3" width="18.25" style="10" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="22" style="10" customWidth="1"/>
-    <col min="6" max="6" width="23.875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="21.625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="82.75" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.875" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="10"/>
+    <col min="5" max="7" width="22" style="10" customWidth="1"/>
+    <col min="8" max="8" width="23.875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="21.625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="82.75" style="10" customWidth="1"/>
+    <col min="11" max="11" width="14.875" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -844,19 +853,25 @@
         <v>5</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
@@ -872,14 +887,16 @@
       <c r="E2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>62</v>
       </c>
@@ -895,14 +912,14 @@
       <c r="E3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>62</v>
       </c>
@@ -918,14 +935,14 @@
       <c r="E4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>71</v>
       </c>
@@ -938,14 +955,14 @@
       <c r="E5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>64</v>
       </c>
@@ -958,17 +975,17 @@
       <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -981,17 +998,17 @@
       <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>74</v>
       </c>
@@ -1004,17 +1021,17 @@
       <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>79</v>
       </c>
@@ -1027,11 +1044,11 @@
       <c r="E9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>81</v>
       </c>
@@ -1044,11 +1061,11 @@
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>82</v>
       </c>
@@ -1061,11 +1078,11 @@
       <c r="E11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="H11" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>83</v>
       </c>
@@ -1078,14 +1095,14 @@
       <c r="E12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
-    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="J8" r:id="rId1"/>
+    <hyperlink ref="J5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1096,13 +1113,13 @@
           <x14:formula1>
             <xm:f>'controlled vocabularies (hide)'!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled vocabularies (hide)'!$D$2:$D$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1121,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1280,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1271,49 +1288,85 @@
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>56</v>
+        <v>85</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1325,7 +1378,7 @@
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1"/>
     <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F8" r:id="rId3" location="categories"/>
+    <hyperlink ref="F10" r:id="rId3" location="categories"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>